<commit_message>
add a new column named routeMap
</commit_message>
<xml_diff>
--- a/roateMap/routeMapData.xlsx
+++ b/roateMap/routeMapData.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="44">
   <si>
-    <t>Route_ID</t>
-  </si>
-  <si>
     <t>Route_Name</t>
   </si>
   <si>
@@ -468,6 +465,11 @@
   </si>
   <si>
     <t>广西</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -822,29 +824,29 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -852,16 +854,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -872,16 +874,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -892,16 +894,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -912,16 +914,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -932,16 +934,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -952,16 +954,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -972,16 +974,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -992,16 +994,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1012,16 +1014,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -1032,16 +1034,16 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1052,16 +1054,16 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -1072,16 +1074,16 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1092,16 +1094,16 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -1112,16 +1114,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1132,16 +1134,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -1152,16 +1154,16 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -1172,16 +1174,16 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1192,16 +1194,16 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -1212,16 +1214,16 @@
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1232,16 +1234,16 @@
         <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -1252,16 +1254,16 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1272,16 +1274,16 @@
         <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23">
         <v>2</v>
@@ -1292,16 +1294,16 @@
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1312,16 +1314,16 @@
         <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -1332,16 +1334,16 @@
         <v>10</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26">
         <v>3</v>

</xml_diff>